<commit_message>
bgmusic-optimize ui-ui responsive mobile
</commit_message>
<xml_diff>
--- a/public/subjects/networking.xlsx
+++ b/public/subjects/networking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Big test\project\public\subjects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phank\OneDrive\Máy tính\Project\Exam Preparation System IT System\project\public\subjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE22100F-9122-4E4A-A92C-F59905C28F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8AD46B-393B-4181-A1F6-2E1AA1A06139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -173,7 +173,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -220,7 +220,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -525,12 +525,12 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,7 +556,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -576,7 +576,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -602,7 +602,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -622,7 +622,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -648,7 +648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -668,7 +668,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -694,7 +694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -714,7 +714,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -740,7 +740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -760,7 +760,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -786,7 +786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -806,7 +806,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -832,7 +832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -852,7 +852,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -878,7 +878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>

</xml_diff>